<commit_message>
fix tariffer and setting docstirngs
</commit_message>
<xml_diff>
--- a/TD-ble-tariffer/RUS/console_app/old_test/0.xlsx
+++ b/TD-ble-tariffer/RUS/console_app/old_test/0.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_07_05 14_49" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="2023_07_05 16_28" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -510,7 +510,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>-74</v>
+        <v>-64</v>
       </c>
       <c r="E2" t="n">
         <v>141</v>
@@ -525,13 +525,13 @@
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>24602</v>
+        <v>24597</v>
       </c>
       <c r="J2" t="n">
-        <v>40357</v>
+        <v>40347</v>
       </c>
       <c r="K2" t="n">
-        <v>24514</v>
+        <v>24509</v>
       </c>
       <c r="L2" t="n">
         <v>1</v>
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>-66</v>
+        <v>-60</v>
       </c>
       <c r="E3" t="n">
         <v>141</v>
@@ -561,19 +561,19 @@
         <v>3.7</v>
       </c>
       <c r="G3" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>23779</v>
+        <v>23774</v>
       </c>
       <c r="J3" t="n">
-        <v>38702</v>
+        <v>38688</v>
       </c>
       <c r="K3" t="n">
-        <v>23655</v>
+        <v>23656</v>
       </c>
       <c r="L3" t="n">
         <v>1</v>
@@ -594,7 +594,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>-62</v>
+        <v>-60</v>
       </c>
       <c r="E4" t="n">
         <v>141</v>
@@ -603,16 +603,16 @@
         <v>3.7</v>
       </c>
       <c r="G4" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H4" t="n">
         <v>1</v>
       </c>
       <c r="I4" t="n">
-        <v>24532</v>
+        <v>24526</v>
       </c>
       <c r="J4" t="n">
-        <v>40231</v>
+        <v>40215</v>
       </c>
       <c r="K4" t="n">
         <v>24420</v>
@@ -651,13 +651,13 @@
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>24576</v>
+        <v>24571</v>
       </c>
       <c r="J5" t="n">
-        <v>40313</v>
+        <v>40303</v>
       </c>
       <c r="K5" t="n">
-        <v>24476</v>
+        <v>24471</v>
       </c>
       <c r="L5" t="n">
         <v>1</v>
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>-60</v>
+        <v>-68</v>
       </c>
       <c r="E6" t="n">
         <v>141</v>
@@ -687,19 +687,19 @@
         <v>3.7</v>
       </c>
       <c r="G6" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
       </c>
       <c r="I6" t="n">
-        <v>24476</v>
+        <v>24472</v>
       </c>
       <c r="J6" t="n">
-        <v>40113</v>
+        <v>40101</v>
       </c>
       <c r="K6" t="n">
-        <v>24370</v>
+        <v>24372</v>
       </c>
       <c r="L6" t="n">
         <v>1</v>
@@ -720,7 +720,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>-60</v>
+        <v>-72</v>
       </c>
       <c r="E7" t="n">
         <v>141</v>
@@ -735,13 +735,13 @@
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>24618</v>
+        <v>24616</v>
       </c>
       <c r="J7" t="n">
-        <v>40390</v>
+        <v>40386</v>
       </c>
       <c r="K7" t="n">
-        <v>24530</v>
+        <v>24528</v>
       </c>
       <c r="L7" t="n">
         <v>1</v>
@@ -762,7 +762,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>-64</v>
+        <v>-68</v>
       </c>
       <c r="E8" t="n">
         <v>141</v>
@@ -771,19 +771,19 @@
         <v>3.7</v>
       </c>
       <c r="G8" t="n">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H8" t="n">
         <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>24545</v>
+        <v>24542</v>
       </c>
       <c r="J8" t="n">
-        <v>40250</v>
+        <v>40239</v>
       </c>
       <c r="K8" t="n">
-        <v>24445</v>
+        <v>24448</v>
       </c>
       <c r="L8" t="n">
         <v>1</v>
@@ -804,7 +804,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>-60</v>
+        <v>-74</v>
       </c>
       <c r="E9" t="n">
         <v>141</v>
@@ -819,13 +819,13 @@
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>24210</v>
+        <v>24206</v>
       </c>
       <c r="J9" t="n">
-        <v>39562</v>
+        <v>39554</v>
       </c>
       <c r="K9" t="n">
-        <v>24116</v>
+        <v>24112</v>
       </c>
       <c r="L9" t="n">
         <v>1</v>
@@ -846,7 +846,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>-70</v>
+        <v>-66</v>
       </c>
       <c r="E10" t="n">
         <v>141</v>
@@ -855,16 +855,16 @@
         <v>3.7</v>
       </c>
       <c r="G10" t="n">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>23869</v>
+        <v>23863</v>
       </c>
       <c r="J10" t="n">
-        <v>38878</v>
+        <v>38862</v>
       </c>
       <c r="K10" t="n">
         <v>23757</v>
@@ -888,7 +888,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>-56</v>
+        <v>-68</v>
       </c>
       <c r="E11" t="n">
         <v>141</v>
@@ -903,13 +903,13 @@
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>24315</v>
+        <v>24311</v>
       </c>
       <c r="J11" t="n">
-        <v>39780</v>
+        <v>39772</v>
       </c>
       <c r="K11" t="n">
-        <v>24215</v>
+        <v>24211</v>
       </c>
       <c r="L11" t="n">
         <v>1</v>

</xml_diff>